<commit_message>
Updated content and files
</commit_message>
<xml_diff>
--- a/docs/templates/data_dictionary - template.xlsx
+++ b/docs/templates/data_dictionary - template.xlsx
@@ -1,22 +1,138 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twey\ownCloud\tweyPrivateFolder\harmonizR\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7685F2F-47F4-46F8-B49D-539A5839EA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
+    <sheet name="readme" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label:en</t>
+  </si>
+  <si>
+    <t>valueType</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Column name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Additional information</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>Index to order variables in the table.</t>
+  </si>
+  <si>
+    <t>If not provided, an automatically generated index is used.</t>
+  </si>
+  <si>
+    <t>If not provided, values are copied from the variable 'name'.
+A language can be specified using a language code, such as ‘label:en’ for English or ‘label:fr’ for French. The default is English. 
+Column name can be 'label' with no language code, but this column name in the Variables and Categories sheets should match.</t>
+  </si>
+  <si>
+    <t>Value type of the variable (e.g., text, integer, decimal, boolean, date, datetime).</t>
+  </si>
+  <si>
+    <t>If not provided, the default value is "text". 
+See additional details at https://opaldoc.obiba.org/en/dev/magma-user-guide/value/type.html.</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>This column is required if the Categories table is present. 
+The value must also match a value in the column ‘name’ in the Variables table.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category code value. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short description of the category code value. </t>
+  </si>
+  <si>
+    <t>Boolean value indicating if the category value in ‘name’ is interpreted as a missing value.</t>
+  </si>
+  <si>
+    <t>Can be in format TRUE/FALSE or 1/0. 
+E.g., "TRUE" for categories "Prefer not to answer” or "Valid skip".</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Name of the variable.</t>
+  </si>
+  <si>
+    <t>Short description of the variable.</t>
+  </si>
+  <si>
+    <t>Name of the variable to which the category belongs.</t>
+  </si>
+  <si>
+    <t>This column is required if the table Categories is present. 
+The combination of ‘variable’ and ‘name’ within the Categories table (i.e., the combination of variable and category code value) must be unique.</t>
+  </si>
+  <si>
+    <t>Must be provided by the user. 
+Each entry must be unique. 
+The first entry is typically the primary identifier variable (e.g., participant unique ID).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The table below provides guidance on using this template. The columns included in the template represent the recommended minimum columns and must have the names as presented for use in Rmonize functions. Additional columns with different names can be present but are not used in data processing. </t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -49,14 +165,179 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -64,13 +345,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -108,7 +397,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -142,6 +431,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -176,9 +466,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -351,62 +642,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>label:en</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>valueType</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>part_id</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>id of the participant</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>cat_example</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Categorical variable. See 'Categories'</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>integer</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -415,96 +674,218 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>label:en</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>missing</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>cat_example</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>First category</t>
-        </is>
-      </c>
-      <c r="D2" t="b">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>cat_example</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Second category</t>
-        </is>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>cat_example</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>-77</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Missing category (Do not want to answer, skip pattern, etc.)</t>
-        </is>
-      </c>
-      <c r="D4" t="b">
+      <c r="C1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B583F2-1C87-427A-976D-54E13CD3FE9A}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>